<commit_message>
Improve CJIS depth management
</commit_message>
<xml_diff>
--- a/tools/cjis/cjis-policy-5.9.4.xlsx
+++ b/tools/cjis/cjis-policy-5.9.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/cjis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D549E8-D37F-F144-B195-3548513563B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC0F3A9-CC73-0245-92EC-5B8B5210A4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3860" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3034" uniqueCount="1633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="1633">
   <si>
     <t>assessable</t>
   </si>
@@ -5437,8 +5437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1653"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A1618" zoomScale="179" workbookViewId="0">
+      <selection activeCell="D1649" sqref="D1649"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5780,9 +5780,6 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
       <c r="B32">
         <v>3</v>
       </c>
@@ -5795,7 +5792,7 @@
         <v>6</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
         <v>36</v>
@@ -5806,7 +5803,7 @@
         <v>6</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
         <v>37</v>
@@ -5817,7 +5814,7 @@
         <v>6</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E35" t="s">
         <v>38</v>
@@ -5828,7 +5825,7 @@
         <v>6</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E36" t="s">
         <v>39</v>
@@ -5839,7 +5836,7 @@
         <v>6</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E37" t="s">
         <v>40</v>
@@ -5850,7 +5847,7 @@
         <v>6</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E38" t="s">
         <v>41</v>
@@ -5861,7 +5858,7 @@
         <v>6</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E39" t="s">
         <v>42</v>
@@ -5872,7 +5869,7 @@
         <v>6</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
         <v>43</v>
@@ -5883,7 +5880,7 @@
         <v>6</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
         <v>44</v>
@@ -5894,7 +5891,7 @@
         <v>6</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E42" t="s">
         <v>45</v>
@@ -5909,9 +5906,6 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>6</v>
-      </c>
       <c r="B44">
         <v>3</v>
       </c>
@@ -5924,7 +5918,7 @@
         <v>6</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E45" t="s">
         <v>48</v>
@@ -5935,7 +5929,7 @@
         <v>6</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E46" t="s">
         <v>49</v>
@@ -5946,7 +5940,7 @@
         <v>6</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E47" t="s">
         <v>50</v>
@@ -5957,7 +5951,7 @@
         <v>6</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E48" t="s">
         <v>51</v>
@@ -5972,9 +5966,6 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>6</v>
-      </c>
       <c r="B50">
         <v>3</v>
       </c>
@@ -5987,7 +5978,7 @@
         <v>6</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E51" t="s">
         <v>54</v>
@@ -5998,7 +5989,7 @@
         <v>6</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E52" t="s">
         <v>55</v>
@@ -6009,7 +6000,7 @@
         <v>6</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E53" t="s">
         <v>56</v>
@@ -6020,7 +6011,7 @@
         <v>6</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E54" t="s">
         <v>57</v>
@@ -6031,7 +6022,7 @@
         <v>6</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E55" t="s">
         <v>58</v>
@@ -6046,9 +6037,6 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>6</v>
-      </c>
       <c r="B57">
         <v>3</v>
       </c>
@@ -6061,7 +6049,7 @@
         <v>6</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E58" t="s">
         <v>61</v>
@@ -6072,7 +6060,7 @@
         <v>6</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E59" t="s">
         <v>62</v>
@@ -6083,7 +6071,7 @@
         <v>6</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E60" t="s">
         <v>63</v>
@@ -6094,7 +6082,7 @@
         <v>6</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E61" t="s">
         <v>64</v>
@@ -6105,7 +6093,7 @@
         <v>6</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E62" t="s">
         <v>65</v>
@@ -6116,7 +6104,7 @@
         <v>6</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E63" t="s">
         <v>66</v>
@@ -6127,7 +6115,7 @@
         <v>6</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E64" t="s">
         <v>67</v>
@@ -6634,9 +6622,6 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>6</v>
-      </c>
       <c r="B114">
         <v>3</v>
       </c>
@@ -6649,7 +6634,7 @@
         <v>6</v>
       </c>
       <c r="B115">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E115" t="s">
         <v>118</v>
@@ -6660,7 +6645,7 @@
         <v>6</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E116" t="s">
         <v>119</v>
@@ -6671,7 +6656,7 @@
         <v>6</v>
       </c>
       <c r="B117">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E117" t="s">
         <v>120</v>
@@ -6682,7 +6667,7 @@
         <v>6</v>
       </c>
       <c r="B118">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E118" t="s">
         <v>121</v>
@@ -6693,7 +6678,7 @@
         <v>6</v>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E119" t="s">
         <v>122</v>
@@ -6704,7 +6689,7 @@
         <v>6</v>
       </c>
       <c r="B120">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E120" t="s">
         <v>123</v>
@@ -6715,7 +6700,7 @@
         <v>6</v>
       </c>
       <c r="B121">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E121" t="s">
         <v>124</v>
@@ -6726,7 +6711,7 @@
         <v>6</v>
       </c>
       <c r="B122">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E122" t="s">
         <v>125</v>
@@ -6737,7 +6722,7 @@
         <v>6</v>
       </c>
       <c r="B123">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E123" t="s">
         <v>126</v>
@@ -6748,7 +6733,7 @@
         <v>6</v>
       </c>
       <c r="B124">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E124" t="s">
         <v>127</v>
@@ -6759,7 +6744,7 @@
         <v>6</v>
       </c>
       <c r="B125">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E125" t="s">
         <v>128</v>
@@ -17795,9 +17780,6 @@
       </c>
     </row>
     <row r="1178" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1178" t="s">
-        <v>6</v>
-      </c>
       <c r="B1178">
         <v>3</v>
       </c>
@@ -17810,7 +17792,7 @@
         <v>6</v>
       </c>
       <c r="B1179">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1179" t="s">
         <v>1157</v>
@@ -17821,7 +17803,7 @@
         <v>6</v>
       </c>
       <c r="B1180">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1180" t="s">
         <v>1158</v>
@@ -17832,7 +17814,7 @@
         <v>6</v>
       </c>
       <c r="B1181">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1181" t="s">
         <v>1159</v>
@@ -17843,7 +17825,7 @@
         <v>6</v>
       </c>
       <c r="B1182">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1182" t="s">
         <v>1160</v>
@@ -18211,9 +18193,6 @@
       </c>
     </row>
     <row r="1218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1218" t="s">
-        <v>6</v>
-      </c>
       <c r="B1218">
         <v>3</v>
       </c>
@@ -18226,7 +18205,7 @@
         <v>6</v>
       </c>
       <c r="B1219">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1219" t="s">
         <v>1197</v>
@@ -18237,7 +18216,7 @@
         <v>6</v>
       </c>
       <c r="B1220">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1220" t="s">
         <v>1198</v>
@@ -18820,9 +18799,6 @@
       </c>
     </row>
     <row r="1275" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1275" t="s">
-        <v>6</v>
-      </c>
       <c r="B1275">
         <v>3</v>
       </c>
@@ -18835,7 +18811,7 @@
         <v>6</v>
       </c>
       <c r="B1276">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1276" t="s">
         <v>1254</v>
@@ -18846,7 +18822,7 @@
         <v>6</v>
       </c>
       <c r="B1277">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1277" t="s">
         <v>1255</v>
@@ -18857,7 +18833,7 @@
         <v>6</v>
       </c>
       <c r="B1278">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1278" t="s">
         <v>1256</v>
@@ -18868,7 +18844,7 @@
         <v>6</v>
       </c>
       <c r="B1279">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1279" t="s">
         <v>1257</v>
@@ -18879,7 +18855,7 @@
         <v>6</v>
       </c>
       <c r="B1280">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1280" t="s">
         <v>1258</v>
@@ -18890,7 +18866,7 @@
         <v>6</v>
       </c>
       <c r="B1281">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1281" t="s">
         <v>1259</v>
@@ -18901,7 +18877,7 @@
         <v>6</v>
       </c>
       <c r="B1282">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1282" t="s">
         <v>1260</v>
@@ -18965,9 +18941,6 @@
       </c>
     </row>
     <row r="1289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1289" t="s">
-        <v>6</v>
-      </c>
       <c r="B1289">
         <v>3</v>
       </c>
@@ -18980,7 +18953,7 @@
         <v>6</v>
       </c>
       <c r="B1290">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1290" t="s">
         <v>1268</v>
@@ -18991,7 +18964,7 @@
         <v>6</v>
       </c>
       <c r="B1291">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1291" t="s">
         <v>1269</v>
@@ -19002,7 +18975,7 @@
         <v>6</v>
       </c>
       <c r="B1292">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1292" t="s">
         <v>1270</v>
@@ -19013,7 +18986,7 @@
         <v>6</v>
       </c>
       <c r="B1293">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1293" t="s">
         <v>1271</v>
@@ -19024,7 +18997,7 @@
         <v>6</v>
       </c>
       <c r="B1294">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1294" t="s">
         <v>1272</v>
@@ -19236,9 +19209,6 @@
       </c>
     </row>
     <row r="1315" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1315" t="s">
-        <v>6</v>
-      </c>
       <c r="B1315">
         <v>3</v>
       </c>
@@ -19251,7 +19221,7 @@
         <v>6</v>
       </c>
       <c r="B1316">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1316" t="s">
         <v>1294</v>
@@ -19262,7 +19232,7 @@
         <v>6</v>
       </c>
       <c r="B1317">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1317" t="s">
         <v>1295</v>
@@ -19273,7 +19243,7 @@
         <v>6</v>
       </c>
       <c r="B1318">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1318" t="s">
         <v>1296</v>
@@ -19284,7 +19254,7 @@
         <v>6</v>
       </c>
       <c r="B1319">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1319" t="s">
         <v>1297</v>
@@ -19295,7 +19265,7 @@
         <v>6</v>
       </c>
       <c r="B1320">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1320" t="s">
         <v>1298</v>
@@ -19306,7 +19276,7 @@
         <v>6</v>
       </c>
       <c r="B1321">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1321" t="s">
         <v>1299</v>
@@ -19317,7 +19287,7 @@
         <v>6</v>
       </c>
       <c r="B1322">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1322" t="s">
         <v>1300</v>
@@ -19328,7 +19298,7 @@
         <v>6</v>
       </c>
       <c r="B1323">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1323" t="s">
         <v>1301</v>

</xml_diff>